<commit_message>
add sleep and walk up
</commit_message>
<xml_diff>
--- a/linux_older.xlsx
+++ b/linux_older.xlsx
@@ -1,64 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyk23\Desktop\note_about_linux\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEBCD8F-FBAE-41F9-8147-25F9673B0518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19425" windowHeight="9840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>符号/命令</t>
+  </si>
+  <si>
+    <t>解析</t>
+  </si>
   <si>
     <t>`（上漂号）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>两个上漂号之间，可以写命令，之后执行，如`ls` =ls</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>符号/命令</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>dkpg（package manager for Debian）</t>
   </si>
   <si>
-    <t>解析</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>是 Debian 和基于 Debian 的系统中一个主要的包管理工具，可以用来安装、构建、卸载、管理 deb 格式的软件包。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apt-get remove </t>
+  </si>
+  <si>
+    <t xml:space="preserve">会删除软件包而保留软件的配置文件
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apt-get purge </t>
+  </si>
+  <si>
+    <t>会同时清除软件包和软件的配置文件</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -67,20 +70,349 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -88,30 +420,322 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -160,7 +784,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -195,7 +819,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -369,48 +993,67 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" customWidth="1"/>
+    <col min="2" max="2" width="56.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" s="3" customFormat="1" ht="28.5" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="1" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add code about modules and mm
</commit_message>
<xml_diff>
--- a/linux_older.xlsx
+++ b/linux_older.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>符号/命令</t>
   </si>
@@ -75,6 +75,12 @@
 2.如果是shell中等待使用wait，则不会等待调用函数中子任务。在函数中使用wait，则只等待函数中启动的后台子任务。
 3.在shell中使用wait命令，相当于高级语言里的多线程同步。
 wait(参数)   使用 wait 是在等待上一批或上一个脚本执行完（即上一个的进程终止），再执行wait之后的命令。</t>
+  </si>
+  <si>
+    <t>dmesg</t>
+  </si>
+  <si>
+    <t>dmesg用来显示内核环缓冲区（kernel-ring buffer）内容，内核将各种消息存放在这里。在系统引导时，内核将与硬件和模块初始化相关的信息填到这个缓冲区中。内核环缓冲区中的消息对于诊断系统问题 通常非常有用。在运行dmesg时，它显示大量信息。通常通过less或grep使用管道查看dmesg的输出，这样可以更容易找到待查信息。</t>
   </si>
 </sst>
 </file>
@@ -82,10 +88,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -105,14 +111,76 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,14 +195,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -143,82 +211,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,9 +232,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,187 +263,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,6 +454,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -490,26 +522,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,19 +549,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -554,10 +560,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -566,133 +572,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1050,10 +1056,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
@@ -1134,6 +1140,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add device driver match
</commit_message>
<xml_diff>
--- a/linux_older.xlsx
+++ b/linux_older.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>符号/命令</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>sudo  echo a &gt; 1.txt 原因是sudo对echo起作用了，但是对后面的 &gt; 命令没有起作用。</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>nm命令主要是用来列出某些文件中的符号（说白了就是一些函数和全局变量等）</t>
   </si>
 </sst>
 </file>
@@ -149,7 +155,129 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,128 +290,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -294,55 +300,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,127 +480,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,48 +496,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,11 +522,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,6 +543,21 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,16 +576,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -603,19 +609,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -624,112 +630,112 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1094,10 +1100,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
@@ -1218,6 +1224,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>